<commit_message>
Separate components in classes, change some structures to improve performance, measure time to execute each class, finish components definition
</commit_message>
<xml_diff>
--- a/Components/components.xlsx
+++ b/Components/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\CEFET\2021_1\Energia solar\Atividades\Atividade 6\trabalho_solar\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599878DA-F9EE-4E31-811E-DFC543C5C34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D5D676-21E6-4577-BAF8-45D7109AB8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{724712C6-E730-4E4D-A874-095120792026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{724712C6-E730-4E4D-A874-095120792026}"/>
   </bookViews>
   <sheets>
     <sheet name="battery" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>discharge_depth_pd</t>
   </si>
   <si>
-    <t>paralel_controlers</t>
-  </si>
-  <si>
     <t>v_min</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>red2</t>
+  </si>
+  <si>
+    <t>parallel_controllers</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8EC5AA-DB69-4B21-9DC1-C8289E29BB61}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6E94EA-1710-4DE4-AE24-921CA066B83C}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +650,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>51.2</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>1160</v>
@@ -729,7 +729,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <v>45</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>330</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>8.8800000000000008</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>37.200000000000003</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>7.66</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>41.9</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>-0.31</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
         <v>5.2999999999999999E-2</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
         <v>0.75</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>

</xml_diff>

<commit_message>
Create classes to deal with specific components, edit default input data
</commit_message>
<xml_diff>
--- a/Components/components.xlsx
+++ b/Components/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\CEFET\2021_1\Energia solar\Atividades\Atividade 6\trabalho_solar\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D5D676-21E6-4577-BAF8-45D7109AB8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25BD666-A4F4-4F20-9018-A31FAFBD1CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{724712C6-E730-4E4D-A874-095120792026}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>v_max</t>
   </si>
   <si>
-    <t>i_load</t>
-  </si>
-  <si>
     <t>p_max</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>v_pmax</t>
   </si>
   <si>
-    <t>i_cc</t>
-  </si>
-  <si>
     <t>v_oc</t>
   </si>
   <si>
@@ -143,6 +137,12 @@
   </si>
   <si>
     <t>parallel_controllers</t>
+  </si>
+  <si>
+    <t>i_sc</t>
+  </si>
+  <si>
+    <t>i_ctl</t>
   </si>
 </sst>
 </file>
@@ -178,9 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -619,7 +622,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +653,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -674,7 +677,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -682,7 +685,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>1160</v>
@@ -729,7 +732,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +763,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -768,7 +771,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>45</v>
@@ -776,7 +779,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>330</v>
@@ -784,7 +787,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>8.8800000000000008</v>
@@ -792,15 +795,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1">
         <v>37.200000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
+      <c r="A9" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B9" s="1">
         <v>7.66</v>
@@ -808,7 +811,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1">
         <v>41.9</v>
@@ -816,7 +819,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1">
         <v>-0.31</v>
@@ -824,7 +827,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1">
         <v>5.2999999999999999E-2</v>
@@ -832,6 +835,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -863,7 +867,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>0.75</v>
@@ -871,7 +875,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>

</xml_diff>